<commit_message>
sync: Sincronización completa antes de push forzado - todos los cambios locales
</commit_message>
<xml_diff>
--- a/PLAN_DE_ACCION.xlsx
+++ b/PLAN_DE_ACCION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\CONDOR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{069E9F87-3D52-4EAE-9B18-DE5924463395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{44AA6EDB-B447-408D-9041-10955A5C4D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{0EEFFD60-9813-4B88-A6E4-C4DF995BC5F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{65274A2D-1DB8-4BD5-87D2-874DD4EAEA51}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de AcciÃ³n" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
   <si>
     <t>Fase</t>
   </si>
@@ -53,154 +53,151 @@
     <t>Fecha Realizada</t>
   </si>
   <si>
-    <t>**Fase 0: Fundación y Arquitectura**</t>
-  </si>
-  <si>
-    <t>**Definición de Arquitectura**</t>
+    <t>Fase 0: Fundación y Arquitectura</t>
+  </si>
+  <si>
+    <t>Definición de Arquitectura</t>
   </si>
   <si>
     <t>Establecer la arquitectura de 3 capas, Inversión de Dependencias (DI) y Principio de Responsabilidad Única (SRP).</t>
   </si>
   <si>
-    <t>**Creación del CLI**</t>
-  </si>
-  <si>
-    <t>Desarrollo de la herramienta `condor_cli.vbs` para automatizar la reconstrucción, testing y exportación de módulos.</t>
-  </si>
-  <si>
-    <t>**Framework de Testing**</t>
-  </si>
-  <si>
-    <t>Implementación del motor de pruebas (`modTestRunner`), la librería de aserciones (`modAssert`) y el patrón de Mocks.</t>
-  </si>
-  <si>
-    <t>**Documentación Inicial**</t>
-  </si>
-  <si>
-    <t>Creación de `CONDOR_MASTER_PLAN.md` y `Lecciones_aprendidas.md` como fuentes de verdad del proyecto.</t>
-  </si>
-  <si>
-    <t>**Fase 1: Servicios de Infraestructura**</t>
-  </si>
-  <si>
-    <t>**Servicio de Configuración**</t>
-  </si>
-  <si>
-    <t>Implementación de `IConfig` / `CConfig` para gestionar la configuración de la aplicación de forma centralizada.</t>
-  </si>
-  <si>
-    <t>**Servicio de Errores**</t>
-  </si>
-  <si>
-    <t>Creación de `IErrorHandlerService` para un manejo de errores robusto y centralizado.</t>
-  </si>
-  <si>
-    <t>**Servicio de Autenticación**</t>
-  </si>
-  <si>
-    <t>Desarrollo de `IAuthService` y su integración con la base de datos "Lanzadera" para la gestión de usuarios y roles.</t>
-  </si>
-  <si>
-    <t>**Logging de Operaciones**</t>
-  </si>
-  <si>
-    <t>Implementación de `IOperationLogger` para la auditoría y trazabilidad de las acciones de negocio.</t>
-  </si>
-  <si>
-    <t>**Fase 2: Lógica de Negocio Principal**</t>
-  </si>
-  <si>
-    <t>**Servicio de Expedientes**</t>
-  </si>
-  <si>
-    <t>Creación de `IExpedienteService` y su repositorio para la consulta de expedientes de la base de datos externa.</t>
-  </si>
-  <si>
-    <t>**Servicio de Solicitudes**</t>
-  </si>
-  <si>
-    <t>Desarrollo de `ISolicitudService` y `ISolicitudRepository` para gestionar el ciclo de vida de la entidad principal.</t>
-  </si>
-  <si>
-    <t>**Servicio de Workflow**</t>
-  </si>
-  <si>
-    <t>Implementación de `IWorkflowService` para gestionar las transiciones de estado de las solicitudes según los roles.</t>
-  </si>
-  <si>
-    <t>**Fase 3: Funcionalidades Avanzadas**</t>
-  </si>
-  <si>
-    <t>**Servicio de Mapeo**</t>
-  </si>
-  <si>
-    <t>Creación de `IMapeoRepository` para gestionar el mapeo entre campos de la BD y marcadores en plantillas Word.</t>
-  </si>
-  <si>
-    <t>**Gestor de Word**</t>
-  </si>
-  <si>
-    <t>Implementación de `IWordManager` para la manipulación programática de documentos Word (.docx).</t>
-  </si>
-  <si>
-    <t>**Servicio de Documentos**</t>
-  </si>
-  <si>
-    <t>Desarrollo de `IDocumentService` que orquesta los servicios de Solicitud, Mapeo y Word para generar y leer documentos.</t>
-  </si>
-  <si>
-    <t>**Servicio de Notificaciones**</t>
-  </si>
-  <si>
-    <t>Creación de `INotificationService` para encolar notificaciones asíncronas en la base de datos de correos.</t>
-  </si>
-  <si>
-    <t>**Fase 4: Capa de Presentación y MVP**</t>
-  </si>
-  <si>
-    <t>**Formulario Principal**</t>
+    <t>Creación del CLI</t>
+  </si>
+  <si>
+    <t>Desarrollo de la herramienta condorcli.vbs para automatizar la reconstrucción, testing y exportación de módulos.</t>
+  </si>
+  <si>
+    <t>Framework de Testing</t>
+  </si>
+  <si>
+    <t>Implementación del motor de pruebas (modTestRunner), la librería de aserciones (modAssert) y el patrón de Mocks.</t>
+  </si>
+  <si>
+    <t>Documentación Inicial</t>
+  </si>
+  <si>
+    <t>Creación de CONDORMASTERPLAN.md y Leccionesaprendidas.md como fuentes de verdad del proyecto.</t>
+  </si>
+  <si>
+    <t>Fase 1: Servicios de Infraestructura</t>
+  </si>
+  <si>
+    <t>Servicio de Configuración</t>
+  </si>
+  <si>
+    <t>Implementación de IConfig / CConfig para gestionar la configuración de la aplicación de forma centralizada.</t>
+  </si>
+  <si>
+    <t>Servicio de Errores</t>
+  </si>
+  <si>
+    <t>Creación de IErrorHandlerService para un manejo de errores robusto y centralizado.</t>
+  </si>
+  <si>
+    <t>Servicio de Autenticación</t>
+  </si>
+  <si>
+    <t>Desarrollo de IAuthService y su integración con la base de datos "Lanzadera" para la gestión de usuarios y roles.</t>
+  </si>
+  <si>
+    <t>Logging de Operaciones</t>
+  </si>
+  <si>
+    <t>Implementación de IOperationLogger para la auditoría y trazabilidad de las acciones de negocio.</t>
+  </si>
+  <si>
+    <t>Fase 2: Lógica de Negocio Principal</t>
+  </si>
+  <si>
+    <t>Servicio de Expedientes</t>
+  </si>
+  <si>
+    <t>Creación de IExpedienteService y su repositorio para la consulta de expedientes de la base de datos externa.</t>
+  </si>
+  <si>
+    <t>Servicio de Solicitudes</t>
+  </si>
+  <si>
+    <t>Desarrollo de ISolicitudService y ISolicitudRepository para gestionar el ciclo de vida de la entidad principal.</t>
+  </si>
+  <si>
+    <t>Servicio de Workflow</t>
+  </si>
+  <si>
+    <t>Implementación de IWorkflowService para gestionar las transiciones de estado de las solicitudes según los roles.</t>
+  </si>
+  <si>
+    <t>Fase 3: Funcionalidades Avanzadas</t>
+  </si>
+  <si>
+    <t>Servicio de Mapeo</t>
+  </si>
+  <si>
+    <t>Creación de IMapeoRepository para gestionar el mapeo entre campos de la BD y marcadores en plantillas Word.</t>
+  </si>
+  <si>
+    <t>Gestor de Word</t>
+  </si>
+  <si>
+    <t>Implementación de IWordManager para la manipulación programática de documentos Word (.docx).</t>
+  </si>
+  <si>
+    <t>Servicio de Documentos</t>
+  </si>
+  <si>
+    <t>Desarrollo de IDocumentService que orquesta los servicios de Solicitud, Mapeo y Word para generar y leer documentos.</t>
+  </si>
+  <si>
+    <t>Servicio de Notificaciones</t>
+  </si>
+  <si>
+    <t>Creación de INotificationService para encolar notificaciones asíncronas en la base de datos de correos.</t>
+  </si>
+  <si>
+    <t>Fase 4: Capa de Presentación y MVP</t>
+  </si>
+  <si>
+    <t>Formulario Principal</t>
   </si>
   <si>
     <t>Creación del panel de control principal que actúa como menú y punto de entrada a las funcionalidades.</t>
   </si>
   <si>
-    <t>**Formulario "Bandeja de Tareas"**</t>
+    <t>Formulario "Bandeja de Tareas"</t>
   </si>
   <si>
     <t>Diseño de la vista que lista las solicitudes pendientes, filtradas según el rol del usuario (Calidad, Técnico).</t>
   </si>
   <si>
-    <t>**Formulario de Solicitud (Alta/Edición)**</t>
+    <t>Formulario de Solicitud (Alta/Edición)</t>
   </si>
   <si>
     <t>Desarrollo del formulario principal para crear y modificar solicitudes, con secciones dinámicas para PC, CD-CA y CD-CA-SUB.</t>
   </si>
   <si>
-    <t>**Integración UI-Backend**</t>
+    <t>Integración UI-Backend</t>
   </si>
   <si>
     <t>Conectar los eventos y controles de todos los formularios con los métodos correspondientes de los servicios VBA.</t>
   </si>
   <si>
-    <t>**Pruebas de Integración E2E**</t>
+    <t>Pruebas de Integración E2E</t>
   </si>
   <si>
     <t>Ejecución de pruebas completas que simulan el flujo de trabajo real del usuario a través de la interfaz.</t>
   </si>
   <si>
-    <t>**HITO: Entrega de MVP para Iteración**</t>
-  </si>
-  <si>
-    <t>**Paquetización y entrega de la primera versión funcional al cliente para iniciar la fase de validación y feedback.**</t>
-  </si>
-  <si>
-    <t>**31/10/2025**</t>
-  </si>
-  <si>
-    <t>**Fase 5: Iteración con Cliente y Estabilización**</t>
-  </si>
-  <si>
-    <t>**Ciclo de Feedback 1**</t>
+    <t>HITO: Entrega de MVP para Iteración</t>
+  </si>
+  <si>
+    <t>Paquetización y entrega de la primera versión funcional al cliente para iniciar la fase de validación y feedback.</t>
+  </si>
+  <si>
+    <t>Fase 5: Iteración con Cliente y Estabilización</t>
+  </si>
+  <si>
+    <t>Ciclo de Feedback 1</t>
   </si>
   <si>
     <t>Recopilación y priorización del feedback inicial del cliente.</t>
@@ -209,7 +206,7 @@
     <t>01/11/2025 - 15/11/2025</t>
   </si>
   <si>
-    <t>**Sprint de Ajustes 1**</t>
+    <t>Sprint de Ajustes 1</t>
   </si>
   <si>
     <t>Implementación de las correcciones y mejoras priorizadas.</t>
@@ -218,7 +215,7 @@
     <t>16/11/2025 - 30/11/2025</t>
   </si>
   <si>
-    <t>**Ciclo de Feedback 2**</t>
+    <t>Ciclo de Feedback 2</t>
   </si>
   <si>
     <t>Nueva ronda de validación con el cliente.</t>
@@ -227,7 +224,7 @@
     <t>01/12/2025 - 10/12/2025</t>
   </si>
   <si>
-    <t>**Sprint de Ajustes 2**</t>
+    <t>Sprint de Ajustes 2</t>
   </si>
   <si>
     <t>Implementación de las mejoras finales.</t>
@@ -236,28 +233,25 @@
     <t>11/12/2025 - 22/12/2025</t>
   </si>
   <si>
-    <t>**Fase 6: Cierre y Entrega Final**</t>
-  </si>
-  <si>
-    <t>**Pruebas de Regresión Finales**</t>
+    <t>Fase 6: Cierre y Entrega Final</t>
+  </si>
+  <si>
+    <t>Pruebas de Regresión Finales</t>
   </si>
   <si>
     <t>Ejecución completa de toda la suite de pruebas para asegurar la estabilidad de la versión final.</t>
   </si>
   <si>
-    <t>**Documentación de Entrega**</t>
+    <t>Documentación de Entrega</t>
   </si>
   <si>
     <t>Preparación de la documentación final para el usuario y el despliegue.</t>
   </si>
   <si>
-    <t>**HITO: Entrega Final del Proyecto**</t>
-  </si>
-  <si>
-    <t>**Entrega de la versión 1.0 del software CONDOR al cliente.**</t>
-  </si>
-  <si>
-    <t>**31/12/2025**</t>
+    <t>HITO: Entrega Final del Proyecto</t>
+  </si>
+  <si>
+    <t>Entrega de la versión 1.0 del software CONDOR al cliente.</t>
   </si>
 </sst>
 </file>
@@ -647,15 +641,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{179C3AAE-381C-4759-97FA-5876C46D3C9D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E4BA66-DD22-4310-AFFC-974BD8560D27}">
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="113.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -998,75 +992,75 @@
       <c r="C22" t="s">
         <v>51</v>
       </c>
-      <c r="D22" t="s">
-        <v>52</v>
+      <c r="D22" s="2">
+        <v>45961</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
         <v>53</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>54</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>55</v>
-      </c>
-      <c r="D23" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
         <v>57</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>58</v>
-      </c>
-      <c r="D24" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
         <v>60</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>61</v>
-      </c>
-      <c r="D25" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" t="s">
         <v>63</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>64</v>
-      </c>
-      <c r="D26" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" t="s">
         <v>66</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>67</v>
-      </c>
-      <c r="C27" t="s">
-        <v>68</v>
       </c>
       <c r="D27" s="2">
         <v>46020</v>
@@ -1074,13 +1068,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" t="s">
         <v>69</v>
-      </c>
-      <c r="C28" t="s">
-        <v>70</v>
       </c>
       <c r="D28" s="2">
         <v>46021</v>
@@ -1088,16 +1082,16 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" t="s">
         <v>71</v>
       </c>
-      <c r="C29" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" t="s">
-        <v>73</v>
+      <c r="D29" s="2">
+        <v>46022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>